<commit_message>
- fixed Expanded Element allow selection of already acquired elements - fixed Venom Infusion context data - updated kineticist tree
</commit_message>
<xml_diff>
--- a/step-level-progression-preview.xlsx
+++ b/step-level-progression-preview.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25028"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dominik.zeising\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dominik.zeising\Desktop\PRD\Github\DarkCodex\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{19760662-3F4F-4467-AA33-68B257B4CC20}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC987820-B348-4559-B7AF-66FB5911936E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7350" yWindow="2880" windowWidth="21600" windowHeight="12855" xr2:uid="{C6E07DBE-61ED-4581-9FBD-188686DA494C}"/>
+    <workbookView xWindow="3165" yWindow="1275" windowWidth="23610" windowHeight="13935" xr2:uid="{C6E07DBE-61ED-4581-9FBD-188686DA494C}"/>
   </bookViews>
   <sheets>
     <sheet name="BlueprintAbilityResource" sheetId="1" r:id="rId1"/>
@@ -125,14 +125,7 @@
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="3">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B0F0"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="2">
     <dxf>
       <fill>
         <patternFill>
@@ -460,7 +453,7 @@
   <dimension ref="A1:G21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>